<commit_message>
fixed r values matched to questions
</commit_message>
<xml_diff>
--- a/Jupyter Notebook/BTC Anlys 20180428 satisfaction r value only.xlsx
+++ b/Jupyter Notebook/BTC Anlys 20180428 satisfaction r value only.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bryan/Dropbox/GitHub/spring-2018-final-projects-bretbryan-wt/Jupyter Notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E70C519-AA54-1649-B872-C848ADF00E31}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD78AFE-7A9E-474F-A6A5-2091E7548E51}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="24600" windowHeight="15540" xr2:uid="{D5192360-7406-454D-866B-A8A89EF9EB09}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>Q02_Program_Start_YearOpenEnded_Response</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Q03_I_would_describe_myself_asResourceful</t>
   </si>
@@ -96,9 +93,6 @@
     <t>Q25_andI_felt_safe_in_my_country_of_service</t>
   </si>
   <si>
-    <t>A02_Satisfaction</t>
-  </si>
-  <si>
     <t>Q28_WorldTeacha_Offered_a_useful_service_to_the_host_country</t>
   </si>
   <si>
@@ -142,6 +136,111 @@
   </si>
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>Q03</t>
+  </si>
+  <si>
+    <t>Q08</t>
+  </si>
+  <si>
+    <t>Q09</t>
+  </si>
+  <si>
+    <t>Q07</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q06</t>
+  </si>
+  <si>
+    <t>Q04</t>
+  </si>
+  <si>
+    <t>Q31</t>
+  </si>
+  <si>
+    <t>Q05</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>Q25</t>
+  </si>
+  <si>
+    <t>Q32</t>
+  </si>
+  <si>
+    <t>Q24</t>
+  </si>
+  <si>
+    <t>Q28</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q29</t>
+  </si>
+  <si>
+    <t>Q36</t>
+  </si>
+  <si>
+    <t>Q23</t>
+  </si>
+  <si>
+    <t>Q30</t>
+  </si>
+  <si>
+    <t>Q34</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>Q38</t>
+  </si>
+  <si>
+    <t>Q33</t>
+  </si>
+  <si>
+    <t>Q18</t>
+  </si>
+  <si>
+    <t>Q22</t>
+  </si>
+  <si>
+    <t>Q39_useful_during_my_year_of_serviceEndofService</t>
+  </si>
+  <si>
+    <t>Q39</t>
+  </si>
+  <si>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>Q35</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q21</t>
+  </si>
+  <si>
+    <t>Q37</t>
   </si>
 </sst>
 </file>
@@ -496,35 +595,34 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2.8895123116067147E-2</v>
+        <v>2.8895123116067099E-2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="str">
-        <f>LEFT(B2,3)</f>
-        <v>Q02</v>
+      <c r="C2" t="s">
+        <v>37</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -537,9 +635,8 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="str">
-        <f>LEFT(B3,3)</f>
-        <v>Q07</v>
+      <c r="C3" t="s">
+        <v>38</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -552,9 +649,8 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="str">
-        <f>LEFT(B4,3)</f>
-        <v>Q08</v>
+      <c r="C4" t="s">
+        <v>39</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -567,9 +663,8 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="str">
-        <f>LEFT(B5,3)</f>
-        <v>Q06</v>
+      <c r="C5" t="s">
+        <v>40</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -582,9 +677,8 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="str">
-        <f>LEFT(B6,3)</f>
-        <v>Q10</v>
+      <c r="C6" t="s">
+        <v>41</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -597,9 +691,8 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="str">
-        <f>LEFT(B7,3)</f>
-        <v>Q05</v>
+      <c r="C7" t="s">
+        <v>42</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -612,9 +705,8 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="str">
-        <f>LEFT(B8,3)</f>
-        <v>Q03</v>
+      <c r="C8" t="s">
+        <v>43</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -625,11 +717,10 @@
         <v>0.19640183314582818</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="str">
-        <f>LEFT(B9,3)</f>
-        <v>Q30</v>
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -642,9 +733,8 @@
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="str">
-        <f>LEFT(B10,3)</f>
-        <v>Q04</v>
+      <c r="C10" t="s">
+        <v>45</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -657,9 +747,8 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="str">
-        <f>LEFT(B11,3)</f>
-        <v>Q12</v>
+      <c r="C11" t="s">
+        <v>46</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -672,9 +761,8 @@
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="str">
-        <f>LEFT(B12,3)</f>
-        <v>Q24</v>
+      <c r="C12" t="s">
+        <v>47</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -685,11 +773,10 @@
         <v>0.30525648354024904</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="str">
-        <f>LEFT(B13,3)</f>
-        <v>Q31</v>
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -702,9 +789,8 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="str">
-        <f>LEFT(B14,3)</f>
-        <v>Q23</v>
+      <c r="C14" t="s">
+        <v>49</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -715,11 +801,10 @@
         <v>0.3132156708043034</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="str">
-        <f>LEFT(B15,3)</f>
-        <v>A02</v>
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -732,9 +817,8 @@
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="str">
-        <f>LEFT(B16,3)</f>
-        <v>Q11</v>
+      <c r="C16" t="s">
+        <v>51</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -745,11 +829,10 @@
         <v>0.33917794718479954</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="str">
-        <f>LEFT(B17,3)</f>
-        <v>Q28</v>
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -760,11 +843,10 @@
         <v>0.36635231482664288</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="str">
-        <f>LEFT(B18,3)</f>
-        <v>Q35</v>
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -777,9 +859,8 @@
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="str">
-        <f>LEFT(B19,3)</f>
-        <v>Q22</v>
+      <c r="C19" t="s">
+        <v>54</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -790,11 +871,10 @@
         <v>0.38342211431296597</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="str">
-        <f>LEFT(B20,3)</f>
-        <v>Q29</v>
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
       </c>
       <c r="D20">
         <v>19</v>
@@ -805,11 +885,10 @@
         <v>0.42715031168230372</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="str">
-        <f>LEFT(B21,3)</f>
-        <v>Q33</v>
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -822,9 +901,8 @@
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" t="str">
-        <f>LEFT(B22,3)</f>
-        <v>Q09</v>
+      <c r="C22" t="s">
+        <v>57</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -837,9 +915,8 @@
       <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" t="str">
-        <f>LEFT(B23,3)</f>
-        <v>Q18</v>
+      <c r="C23" t="s">
+        <v>58</v>
       </c>
       <c r="D23">
         <v>22</v>
@@ -850,11 +927,10 @@
         <v>0.49423904863614904</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="str">
-        <f>LEFT(B24,3)</f>
-        <v>Q37</v>
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
       </c>
       <c r="D24">
         <v>23</v>
@@ -865,11 +941,10 @@
         <v>0.50038696561798757</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="str">
-        <f>LEFT(B25,3)</f>
-        <v>Q32</v>
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
       </c>
       <c r="D25">
         <v>24</v>
@@ -882,9 +957,8 @@
       <c r="B26" t="s">
         <v>15</v>
       </c>
-      <c r="C26" t="str">
-        <f>LEFT(B26,3)</f>
-        <v>Q17</v>
+      <c r="C26" t="s">
+        <v>61</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -897,9 +971,8 @@
       <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C27" t="str">
-        <f>LEFT(B27,3)</f>
-        <v>Q21</v>
+      <c r="C27" t="s">
+        <v>62</v>
       </c>
       <c r="D27">
         <v>26</v>
@@ -910,11 +983,10 @@
         <v>0.52641017794903955</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" t="str">
-        <f>LEFT(B28,3)</f>
-        <v>Q38</v>
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
       </c>
       <c r="D28">
         <v>27</v>
@@ -927,9 +999,8 @@
       <c r="B29" t="s">
         <v>14</v>
       </c>
-      <c r="C29" t="str">
-        <f>LEFT(B29,3)</f>
-        <v>Q16</v>
+      <c r="C29" t="s">
+        <v>65</v>
       </c>
       <c r="D29">
         <v>28</v>
@@ -942,9 +1013,8 @@
       <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="C30" t="str">
-        <f>LEFT(B30,3)</f>
-        <v>Q13</v>
+      <c r="C30" t="s">
+        <v>66</v>
       </c>
       <c r="D30">
         <v>29</v>
@@ -957,9 +1027,8 @@
       <c r="B31" t="s">
         <v>12</v>
       </c>
-      <c r="C31" t="str">
-        <f>LEFT(B31,3)</f>
-        <v>Q14</v>
+      <c r="C31" t="s">
+        <v>67</v>
       </c>
       <c r="D31">
         <v>30</v>
@@ -970,11 +1039,10 @@
         <v>0.62761217459174834</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" t="str">
-        <f>LEFT(B32,3)</f>
-        <v>Q34</v>
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
       </c>
       <c r="D32">
         <v>31</v>
@@ -987,9 +1055,8 @@
       <c r="B33" t="s">
         <v>13</v>
       </c>
-      <c r="C33" t="str">
-        <f>LEFT(B33,3)</f>
-        <v>Q15</v>
+      <c r="C33" t="s">
+        <v>69</v>
       </c>
       <c r="D33">
         <v>32</v>
@@ -1002,9 +1069,8 @@
       <c r="B34" t="s">
         <v>17</v>
       </c>
-      <c r="C34" t="str">
-        <f>LEFT(B34,3)</f>
-        <v>Q20</v>
+      <c r="C34" t="s">
+        <v>70</v>
       </c>
       <c r="D34">
         <v>33</v>
@@ -1012,14 +1078,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>0.69534533912116003</v>
+        <v>0.71425841761180431</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" t="str">
-        <f>LEFT(B35,3)</f>
-        <v>Q25</v>
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
       </c>
       <c r="D35">
         <v>34</v>
@@ -1030,11 +1095,10 @@
         <v>0.71425841761180431</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="str">
-        <f>LEFT(B36,3)</f>
-        <v>Q36</v>
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
       </c>
       <c r="D36">
         <v>35</v>

</xml_diff>